<commit_message>
complete vlookup and lookup function
</commit_message>
<xml_diff>
--- a/MS Excell/for job.xlsx
+++ b/MS Excell/for job.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="relative reference" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,13 @@
     <sheet name="And" sheetId="7" r:id="rId6"/>
     <sheet name="DateFunction" sheetId="8" r:id="rId7"/>
     <sheet name="StatisticalFunction" sheetId="9" r:id="rId8"/>
+    <sheet name="VlookupDataValidationExact" sheetId="11" r:id="rId9"/>
+    <sheet name="VlookupApproximatematch" sheetId="12" r:id="rId10"/>
+    <sheet name="LookupFullRecord" sheetId="13" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="vtable">VlookupDataValidationExact!$A$3:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="167">
   <si>
     <t>Month</t>
   </si>
@@ -327,19 +333,255 @@
   </si>
   <si>
     <t>Count of numbers where they have john &amp; Mon</t>
+  </si>
+  <si>
+    <t>Top Product</t>
+  </si>
+  <si>
+    <t>product code</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Cosmetics</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Perfumes</t>
+  </si>
+  <si>
+    <t>Clothes</t>
+  </si>
+  <si>
+    <t>1000-165-B100</t>
+  </si>
+  <si>
+    <t>1000-165-B101</t>
+  </si>
+  <si>
+    <t>1000-165-B102</t>
+  </si>
+  <si>
+    <t>1000-165-B103</t>
+  </si>
+  <si>
+    <t>1000-165-B104</t>
+  </si>
+  <si>
+    <t>1000-165-B105</t>
+  </si>
+  <si>
+    <t>1000-165-B106</t>
+  </si>
+  <si>
+    <t>1000-165-B107</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Vlookup and data validation with Name range</t>
+  </si>
+  <si>
+    <t>Rules For commission</t>
+  </si>
+  <si>
+    <t>Sales Amount</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Commission paid</t>
+  </si>
+  <si>
+    <t>tk.0 &lt;= sales&lt; tk.2000</t>
+  </si>
+  <si>
+    <t>tk.2000 &lt;= sales&lt; tk.3000</t>
+  </si>
+  <si>
+    <t>tk.3000 &lt;= sales&lt; tk.5000</t>
+  </si>
+  <si>
+    <t>tk.5000&lt;= sales&lt; tk.10000</t>
+  </si>
+  <si>
+    <t>tk.10000 &gt;= sales</t>
+  </si>
+  <si>
+    <t>Fair</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Very Good</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Sales Done</t>
+  </si>
+  <si>
+    <t>Commission Received</t>
+  </si>
+  <si>
+    <t>V= Vertical</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>880-10048</t>
+  </si>
+  <si>
+    <t>880-10049</t>
+  </si>
+  <si>
+    <t>880-10050</t>
+  </si>
+  <si>
+    <t>880-10051</t>
+  </si>
+  <si>
+    <t>880-10052</t>
+  </si>
+  <si>
+    <t>880-10053</t>
+  </si>
+  <si>
+    <t>880-10054</t>
+  </si>
+  <si>
+    <t>880-10055</t>
+  </si>
+  <si>
+    <t>880-10056</t>
+  </si>
+  <si>
+    <t>taj</t>
+  </si>
+  <si>
+    <t>shahid</t>
+  </si>
+  <si>
+    <t>nazrul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rina </t>
+  </si>
+  <si>
+    <t>Nurul</t>
+  </si>
+  <si>
+    <t>Feroza</t>
+  </si>
+  <si>
+    <t>Kohinoor</t>
+  </si>
+  <si>
+    <t>Tahiya</t>
+  </si>
+  <si>
+    <t>khan</t>
+  </si>
+  <si>
+    <t>islam</t>
+  </si>
+  <si>
+    <t>Shekh</t>
+  </si>
+  <si>
+    <t>Begum</t>
+  </si>
+  <si>
+    <t>taj@gmail.com</t>
+  </si>
+  <si>
+    <t>shahid@gmail.com</t>
+  </si>
+  <si>
+    <t>naz@gmail.com</t>
+  </si>
+  <si>
+    <t>017-55455</t>
+  </si>
+  <si>
+    <t>017-55456</t>
+  </si>
+  <si>
+    <t>017-55457</t>
+  </si>
+  <si>
+    <t>017-55458</t>
+  </si>
+  <si>
+    <t>017-55459</t>
+  </si>
+  <si>
+    <t>017-55460</t>
+  </si>
+  <si>
+    <t>017-55461</t>
+  </si>
+  <si>
+    <t>017-55462</t>
+  </si>
+  <si>
+    <t>017-55463</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="dddd"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +642,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -473,11 +723,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -503,6 +755,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,10 +778,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="7" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="7" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -933,6 +1201,377 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="38"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="10">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="10">
+        <v>10000</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="35">
+        <v>4990</v>
+      </c>
+      <c r="B13">
+        <f>VLOOKUP(A13,B3:D8,3,1)</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="str">
+        <f>LOOKUP($A$17,$A$5:$A$13,B5:B13)</f>
+        <v xml:space="preserve">Rina </v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" ref="C17:E17" si="0">LOOKUP($A$17,$A$5:$A$13,C5:C13)</f>
+        <v>Begum</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>taj@gmail.com</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>017-55459</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A17">
+      <formula1>$A$5:$A$13</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D6:D13" r:id="rId2" display="taj@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D7" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
@@ -1098,24 +1737,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -1373,7 +2012,7 @@
       </c>
       <c r="F14" s="11">
         <f ca="1">IF(E4&lt;F4,TODAY(),TODAY()+10)</f>
-        <v>44133</v>
+        <v>44134</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.25">
@@ -1562,10 +2201,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1707,12 +2346,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
@@ -1753,10 +2392,10 @@
         <v>43465</v>
       </c>
       <c r="E8" s="20"/>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="29"/>
+      <c r="I8" s="31"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="17"/>
@@ -1881,7 +2520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1894,16 +2533,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="24" t="s">
         <v>81</v>
       </c>
       <c r="E2">
@@ -2081,4 +2720,197 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="10">
+        <v>20</v>
+      </c>
+      <c r="D4" s="41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="10">
+        <v>25</v>
+      </c>
+      <c r="D5" s="41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="10">
+        <v>30</v>
+      </c>
+      <c r="D6" s="41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="10">
+        <v>40</v>
+      </c>
+      <c r="D7" s="41">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="10">
+        <v>15</v>
+      </c>
+      <c r="D8" s="41">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="10">
+        <v>18</v>
+      </c>
+      <c r="D9" s="41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="10">
+        <v>32</v>
+      </c>
+      <c r="D10" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="10">
+        <v>21</v>
+      </c>
+      <c r="D11" s="41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="35">
+        <f>VLOOKUP(A18,vtable,4,0)</f>
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="33">
+        <f>B18*C18</f>
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:C14"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A18">
+      <formula1>$A$4:$A$11</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
complete protect sheet and page setup
</commit_message>
<xml_diff>
--- a/MS Excell/for job.xlsx
+++ b/MS Excell/for job.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="relative reference" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="VlookupDataValidationExact" sheetId="11" r:id="rId9"/>
     <sheet name="VlookupApproximatematch" sheetId="12" r:id="rId10"/>
     <sheet name="LookupFullRecord" sheetId="13" r:id="rId11"/>
+    <sheet name="HyperlinkToWorksheet" sheetId="14" r:id="rId12"/>
+    <sheet name="HypelinkToFile" sheetId="15" r:id="rId13"/>
+    <sheet name="HyperlinkToWebpage" sheetId="16" r:id="rId14"/>
+    <sheet name="HyperlinkToUpdate" sheetId="17" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="vtable">VlookupDataValidationExact!$A$3:$D$11</definedName>
@@ -66,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="171">
   <si>
     <t>Month</t>
   </si>
@@ -567,6 +571,18 @@
   </si>
   <si>
     <t>017-55463</t>
+  </si>
+  <si>
+    <t>Go to LookupFullRecord</t>
+  </si>
+  <si>
+    <t>Go To</t>
+  </si>
+  <si>
+    <t>Go to webpage</t>
+  </si>
+  <si>
+    <t>click to update</t>
   </si>
 </sst>
 </file>
@@ -579,7 +595,7 @@
     <numFmt numFmtId="165" formatCode="dddd"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -729,7 +745,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -757,6 +773,16 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -778,20 +804,21 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="7" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="7" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -810,6 +837,67 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Smiley Face 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247775" y="695325"/>
+          <a:ext cx="1257300" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="smileyFace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1078,7 +1166,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1294,7 @@
   <dimension ref="A3:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,25 +1307,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="38"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1310,15 +1398,15 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="29" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
+      <c r="A13" s="28">
         <v>4990</v>
       </c>
       <c r="B13">
@@ -1328,6 +1416,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1335,223 +1424,224 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="1" max="1" width="19" style="46" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="46" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="46" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="18" style="46" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="46"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="45" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="46" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="46" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="46" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="46" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="46" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="46" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="46" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="46" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="46" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="45" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="46" t="str">
         <f>LOOKUP($A$17,$A$5:$A$13,B5:B13)</f>
         <v xml:space="preserve">Rina </v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="46" t="str">
         <f t="shared" ref="C17:E17" si="0">LOOKUP($A$17,$A$5:$A$13,C5:C13)</f>
         <v>Begum</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="46" t="str">
         <f t="shared" si="0"/>
         <v>taj@gmail.com</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17" s="46" t="str">
         <f t="shared" si="0"/>
         <v>017-55459</v>
       </c>
@@ -1569,6 +1659,134 @@
     <hyperlink ref="D7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" location="LookupFullRecord!A4" display="Go to LookupFullRecord"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="44"/>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="44"/>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="44"/>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="44"/>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="44"/>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="44"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" tooltip="youtube"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1576,7 +1794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1720,6 +1940,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1727,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,24 +1958,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -1903,7 +2124,13 @@
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.92708333333333337" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;Lpage &amp;P of &amp;N</oddHeader>
+    <firstHeader>&amp;C&amp;G</firstHeader>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1912,7 +2139,7 @@
   <dimension ref="E3:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,7 +2239,7 @@
       </c>
       <c r="F14" s="11">
         <f ca="1">IF(E4&lt;F4,TODAY(),TODAY()+10)</f>
-        <v>44134</v>
+        <v>44135</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.25">
@@ -2029,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,6 +2390,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2171,7 +2399,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,10 +2429,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2325,6 +2553,7 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2332,8 +2561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,12 +2575,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
@@ -2392,10 +2621,10 @@
         <v>43465</v>
       </c>
       <c r="E8" s="20"/>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="17"/>
@@ -2513,6 +2742,12 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="14" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="3" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 
@@ -2521,7 +2756,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D18"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,20 +2970,20 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="31" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2762,7 +2997,7 @@
       <c r="C4" s="10">
         <v>20</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="32">
         <v>26</v>
       </c>
     </row>
@@ -2776,7 +3011,7 @@
       <c r="C5" s="10">
         <v>25</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="32">
         <v>28</v>
       </c>
     </row>
@@ -2790,7 +3025,7 @@
       <c r="C6" s="10">
         <v>30</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="32">
         <v>30</v>
       </c>
     </row>
@@ -2804,7 +3039,7 @@
       <c r="C7" s="10">
         <v>40</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="32">
         <v>31</v>
       </c>
     </row>
@@ -2818,7 +3053,7 @@
       <c r="C8" s="10">
         <v>15</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="32">
         <v>32</v>
       </c>
     </row>
@@ -2832,7 +3067,7 @@
       <c r="C9" s="10">
         <v>18</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="32">
         <v>100</v>
       </c>
     </row>
@@ -2846,7 +3081,7 @@
       <c r="C10" s="10">
         <v>32</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="32">
         <v>4</v>
       </c>
     </row>
@@ -2860,28 +3095,28 @@
       <c r="C11" s="10">
         <v>21</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="32">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="27" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2889,14 +3124,14 @@
       <c r="A18" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="35">
+      <c r="B18" s="28">
         <f>VLOOKUP(A18,vtable,4,0)</f>
         <v>30</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="26">
         <f>B18*C18</f>
         <v>120</v>
       </c>
@@ -2911,6 +3146,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="16383" man="1"/>
+  </rowBreaks>
+  <picture r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complete filtering table subtotal column chart
</commit_message>
<xml_diff>
--- a/MS Excell/for job.xlsx
+++ b/MS Excell/for job.xlsx
@@ -4,26 +4,34 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="relative reference" sheetId="1" r:id="rId1"/>
     <sheet name="Absolute reference" sheetId="2" r:id="rId2"/>
     <sheet name="Mixed reference" sheetId="3" r:id="rId3"/>
-    <sheet name="If" sheetId="5" r:id="rId4"/>
-    <sheet name="NestedIf" sheetId="6" r:id="rId5"/>
-    <sheet name="And" sheetId="7" r:id="rId6"/>
-    <sheet name="DateFunction" sheetId="8" r:id="rId7"/>
-    <sheet name="StatisticalFunction" sheetId="9" r:id="rId8"/>
-    <sheet name="VlookupDataValidationExact" sheetId="11" r:id="rId9"/>
-    <sheet name="VlookupApproximatematch" sheetId="12" r:id="rId10"/>
-    <sheet name="LookupFullRecord" sheetId="13" r:id="rId11"/>
-    <sheet name="HyperlinkToWorksheet" sheetId="14" r:id="rId12"/>
-    <sheet name="HypelinkToFile" sheetId="15" r:id="rId13"/>
-    <sheet name="HyperlinkToWebpage" sheetId="16" r:id="rId14"/>
-    <sheet name="HyperlinkToUpdate" sheetId="17" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId4"/>
+    <sheet name="If" sheetId="5" r:id="rId5"/>
+    <sheet name="NestedIf" sheetId="6" r:id="rId6"/>
+    <sheet name="And" sheetId="7" r:id="rId7"/>
+    <sheet name="DateFunction" sheetId="8" r:id="rId8"/>
+    <sheet name="StatisticalFunction" sheetId="9" r:id="rId9"/>
+    <sheet name="VlookupDataValidationExact" sheetId="11" r:id="rId10"/>
+    <sheet name="subtotal" sheetId="19" r:id="rId11"/>
+    <sheet name="Filtering" sheetId="20" r:id="rId12"/>
+    <sheet name="Chart2" sheetId="24" r:id="rId13"/>
+    <sheet name="ColumnChart" sheetId="22" r:id="rId14"/>
+    <sheet name="TableTotalRow" sheetId="21" r:id="rId15"/>
+    <sheet name="VlookupApproximatematch" sheetId="12" r:id="rId16"/>
+    <sheet name="LookupFullRecord" sheetId="13" r:id="rId17"/>
+    <sheet name="HyperlinkToWorksheet" sheetId="14" r:id="rId18"/>
+    <sheet name="HypelinkToFile" sheetId="15" r:id="rId19"/>
+    <sheet name="HyperlinkToWebpage" sheetId="16" r:id="rId20"/>
+    <sheet name="HyperlinkToUpdate" sheetId="17" r:id="rId21"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Filtering!$B$4:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">VlookupApproximatematch!$A$3:$D$8</definedName>
     <definedName name="vtable">VlookupDataValidationExact!$A$3:$D$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -70,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="181">
   <si>
     <t>Month</t>
   </si>
@@ -583,6 +591,36 @@
   </si>
   <si>
     <t>click to update</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Laptop Total</t>
+  </si>
+  <si>
+    <t>Shoes Total</t>
+  </si>
+  <si>
+    <t>Cosmetics Total</t>
+  </si>
+  <si>
+    <t>Watches Total</t>
+  </si>
+  <si>
+    <t>camera Total</t>
+  </si>
+  <si>
+    <t>Mobile Total</t>
+  </si>
+  <si>
+    <t>Clothes Total</t>
+  </si>
+  <si>
+    <t>Perfumes Total</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -597,7 +635,7 @@
     <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,8 +708,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,8 +766,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -738,6 +796,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -745,7 +899,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -783,6 +937,18 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,18 +973,28 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="6" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -826,7 +1002,220 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -839,7 +1228,2348 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnChart!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>ColumnChart!$B$4:$C$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1000-165-B100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000-165-B101</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1000-165-B102</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1000-165-B103</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1000-165-B104</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1000-165-B105</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000-165-B106</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000-165-B107</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Mobile</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>camera</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Watches</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Cosmetics</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Shoes</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Laptop</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Perfumes</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Clothes</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnChart!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-797E-4493-8780-57DCB9C8FF87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnChart!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>ColumnChart!$B$4:$C$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1000-165-B100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000-165-B101</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1000-165-B102</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1000-165-B103</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1000-165-B104</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1000-165-B105</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000-165-B106</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000-165-B107</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Mobile</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>camera</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Watches</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Cosmetics</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Shoes</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Laptop</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Perfumes</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Clothes</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnChart!$E$4:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-797E-4493-8780-57DCB9C8FF87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="65"/>
+        <c:axId val="1519455375"/>
+        <c:axId val="1519457455"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1519455375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1519457455"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1519457455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1519455375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnChart!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>ColumnChart!$B$4:$C$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1000-165-B100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000-165-B101</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1000-165-B102</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1000-165-B103</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1000-165-B104</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1000-165-B105</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000-165-B106</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000-165-B107</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Mobile</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>camera</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Watches</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Cosmetics</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Shoes</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Laptop</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Perfumes</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Clothes</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnChart!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECDD-4CF7-A0A2-414EB7903513}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnChart!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>ColumnChart!$B$4:$C$11</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1000-165-B100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1000-165-B101</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1000-165-B102</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1000-165-B103</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1000-165-B104</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1000-165-B105</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1000-165-B106</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1000-165-B107</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Mobile</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>camera</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Watches</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Cosmetics</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Shoes</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Laptop</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Perfumes</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Clothes</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnChart!$E$4:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ECDD-4CF7-A0A2-414EB7903513}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1524819151"/>
+        <c:axId val="1524810415"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1524819151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524810415"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1524810415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1524819151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="60" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8667750" cy="6286500"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -898,6 +3628,19 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C4:F13" totalsRowCount="1" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="C4:F12"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Top Product" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="2" name="product code" totalsRowFunction="count" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Quantity" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="Price" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1291,10 +4034,933 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="10">
+        <v>20</v>
+      </c>
+      <c r="D4" s="32">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="10">
+        <v>25</v>
+      </c>
+      <c r="D5" s="32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="10">
+        <v>30</v>
+      </c>
+      <c r="D6" s="32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="10">
+        <v>40</v>
+      </c>
+      <c r="D7" s="32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="10">
+        <v>15</v>
+      </c>
+      <c r="D8" s="32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="10">
+        <v>18</v>
+      </c>
+      <c r="D9" s="32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="10">
+        <v>32</v>
+      </c>
+      <c r="D10" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="10">
+        <v>21</v>
+      </c>
+      <c r="D11" s="32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="28">
+        <f>VLOOKUP(A18,vtable,4,0)</f>
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" s="26">
+        <f>B18*C18</f>
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:C14"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A18">
+      <formula1>$A$4:$A$11</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="13" max="16383" man="1"/>
+  </rowBreaks>
+  <picture r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="10">
+        <v>18</v>
+      </c>
+      <c r="E4" s="32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="32">
+        <f>SUBTOTAL(9,E4:E4)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="10">
+        <v>15</v>
+      </c>
+      <c r="E6" s="32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="32">
+        <f>SUBTOTAL(9,E6:E6)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="10">
+        <v>40</v>
+      </c>
+      <c r="E8" s="32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="32">
+        <f>SUBTOTAL(9,E8:E8)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="10">
+        <v>30</v>
+      </c>
+      <c r="E10" s="32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="32">
+        <f>SUBTOTAL(9,E10:E10)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="10">
+        <v>25</v>
+      </c>
+      <c r="E12" s="32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="32">
+        <f>SUBTOTAL(9,E12:E12)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="10">
+        <v>20</v>
+      </c>
+      <c r="E14" s="32">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="32">
+        <f>SUBTOTAL(9,E14:E14)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="10">
+        <v>21</v>
+      </c>
+      <c r="E16" s="32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="32">
+        <f>SUBTOTAL(9,E16:E16)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="10">
+        <v>32</v>
+      </c>
+      <c r="E18" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51">
+        <f>SUBTOTAL(9,E18:E18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51">
+        <f>SUBTOTAL(9,E4:E18)</f>
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B4:E11">
+    <sortCondition descending="1" ref="E6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="64">
+        <v>20</v>
+      </c>
+      <c r="E4" s="65">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="66">
+        <v>25</v>
+      </c>
+      <c r="E5" s="67">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="64">
+        <v>30</v>
+      </c>
+      <c r="E6" s="65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="66">
+        <v>40</v>
+      </c>
+      <c r="E7" s="67">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="64">
+        <v>15</v>
+      </c>
+      <c r="E8" s="65">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="66">
+        <v>18</v>
+      </c>
+      <c r="E9" s="67">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="64">
+        <v>32</v>
+      </c>
+      <c r="E10" s="65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="66">
+        <v>21</v>
+      </c>
+      <c r="E11" s="67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="68">
+        <f>SUBTOTAL(103,Filtering!$C$4:$C$11)</f>
+        <v>8</v>
+      </c>
+      <c r="D12" s="68">
+        <f>SUBTOTAL(109,Filtering!$D$4:$D$11)</f>
+        <v>201</v>
+      </c>
+      <c r="E12" s="69">
+        <f>SUBTOTAL(109,Filtering!$E$4:$E$11)</f>
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="64">
+        <v>20</v>
+      </c>
+      <c r="E4" s="65">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="66">
+        <v>25</v>
+      </c>
+      <c r="E5" s="67">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="64">
+        <v>30</v>
+      </c>
+      <c r="E6" s="65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="66">
+        <v>40</v>
+      </c>
+      <c r="E7" s="67">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="64">
+        <v>15</v>
+      </c>
+      <c r="E8" s="65">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="66">
+        <v>18</v>
+      </c>
+      <c r="E9" s="67">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="64">
+        <v>32</v>
+      </c>
+      <c r="E10" s="65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="70">
+        <v>21</v>
+      </c>
+      <c r="E11" s="32">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="10">
+        <v>20</v>
+      </c>
+      <c r="F5" s="54">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="10">
+        <v>25</v>
+      </c>
+      <c r="F6" s="54">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="10">
+        <v>30</v>
+      </c>
+      <c r="F7" s="54">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="10">
+        <v>40</v>
+      </c>
+      <c r="F8" s="54">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="10">
+        <v>15</v>
+      </c>
+      <c r="F9" s="54">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="10">
+        <v>18</v>
+      </c>
+      <c r="F10" s="54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="10">
+        <v>32</v>
+      </c>
+      <c r="F11" s="54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="59">
+        <v>21</v>
+      </c>
+      <c r="F12" s="60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="59">
+        <f>SUBTOTAL(103,Table13[product code])</f>
+        <v>8</v>
+      </c>
+      <c r="E13" s="59">
+        <f>SUBTOTAL(109,Table13[Quantity])</f>
+        <v>201</v>
+      </c>
+      <c r="F13" s="61">
+        <f>SUBTOTAL(109,Table13[Price])</f>
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,8 +5025,8 @@
       <c r="A6" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="10">
-        <v>3000</v>
+      <c r="B6" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>123</v>
@@ -1411,16 +5077,17 @@
       </c>
       <c r="B13">
         <f>VLOOKUP(A13,B3:D8,3,1)</f>
-        <v>200</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A3:D8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E17"/>
   <sheetViews>
@@ -1430,218 +5097,218 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" style="46" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="46" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="46" customWidth="1"/>
-    <col min="5" max="5" width="18" style="46" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="46"/>
+    <col min="1" max="1" width="19" style="38" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="18" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="37" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="38" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="38" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="38" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="38" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="38" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="38" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="38" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="38" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="E13" s="46" t="s">
+      <c r="E13" s="38" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="37" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="46" t="str">
+      <c r="B17" s="38" t="str">
         <f>LOOKUP($A$17,$A$5:$A$13,B5:B13)</f>
         <v xml:space="preserve">Rina </v>
       </c>
-      <c r="C17" s="46" t="str">
+      <c r="C17" s="38" t="str">
         <f t="shared" ref="C17:E17" si="0">LOOKUP($A$17,$A$5:$A$13,C5:C13)</f>
         <v>Begum</v>
       </c>
-      <c r="D17" s="46" t="str">
+      <c r="D17" s="38" t="str">
         <f t="shared" si="0"/>
         <v>taj@gmail.com</v>
       </c>
-      <c r="E17" s="46" t="str">
+      <c r="E17" s="38" t="str">
         <f t="shared" si="0"/>
         <v>017-55459</v>
       </c>
@@ -1663,7 +5330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4"/>
   <sheetViews>
@@ -1690,7 +5357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3"/>
   <sheetViews>
@@ -1717,7 +5384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:C9"/>
   <sheetViews>
@@ -1731,27 +5398,27 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="35" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="44"/>
+      <c r="C4" s="36"/>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="44"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="44"/>
+      <c r="C6" s="36"/>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="44"/>
+      <c r="C7" s="36"/>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="44"/>
+      <c r="C8" s="36"/>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="44"/>
+      <c r="C9" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1760,33 +5427,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="34" t="s">
-        <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1944,6 +5584,33 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
@@ -1958,24 +5625,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="8">
@@ -2136,6 +5803,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2239,7 +5918,7 @@
       </c>
       <c r="F14" s="11">
         <f ca="1">IF(E4&lt;F4,TODAY(),TODAY()+10)</f>
-        <v>44135</v>
+        <v>44136</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.25">
@@ -2252,11 +5931,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2394,7 +6073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H12"/>
   <sheetViews>
@@ -2429,10 +6108,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="39"/>
+      <c r="B4" s="45"/>
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2557,7 +6236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J21"/>
   <sheetViews>
@@ -2575,12 +6254,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
@@ -2621,10 +6300,10 @@
         <v>43465</v>
       </c>
       <c r="E8" s="20"/>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="41"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="17"/>
@@ -2751,7 +6430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
@@ -2955,201 +6634,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="26" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="10">
-        <v>20</v>
-      </c>
-      <c r="D4" s="32">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="10">
-        <v>25</v>
-      </c>
-      <c r="D5" s="32">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="10">
-        <v>30</v>
-      </c>
-      <c r="D6" s="32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="10">
-        <v>40</v>
-      </c>
-      <c r="D7" s="32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" s="10">
-        <v>15</v>
-      </c>
-      <c r="D8" s="32">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="10">
-        <v>18</v>
-      </c>
-      <c r="D9" s="32">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="10">
-        <v>32</v>
-      </c>
-      <c r="D10" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="10">
-        <v>21</v>
-      </c>
-      <c r="D11" s="32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="28">
-        <f>VLOOKUP(A18,vtable,4,0)</f>
-        <v>30</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18" s="26">
-        <f>B18*C18</f>
-        <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A14:C14"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A18">
-      <formula1>$A$4:$A$11</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="13" max="16383" man="1"/>
-  </rowBreaks>
-  <picture r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
complete pivot table pivot chart consoladitaion
</commit_message>
<xml_diff>
--- a/MS Excell/for job.xlsx
+++ b/MS Excell/for job.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="relative reference" sheetId="1" r:id="rId1"/>
@@ -23,21 +23,38 @@
     <sheet name="ColumnChart" sheetId="22" r:id="rId14"/>
     <sheet name="Chart1" sheetId="26" r:id="rId15"/>
     <sheet name="pieBarLineChart" sheetId="25" r:id="rId16"/>
-    <sheet name="TableTotalRow" sheetId="21" r:id="rId17"/>
-    <sheet name="VlookupApproximatematch" sheetId="12" r:id="rId18"/>
-    <sheet name="LookupFullRecord" sheetId="13" r:id="rId19"/>
-    <sheet name="HyperlinkToWorksheet" sheetId="14" r:id="rId20"/>
-    <sheet name="HypelinkToFile" sheetId="15" r:id="rId21"/>
-    <sheet name="HyperlinkToWebpage" sheetId="16" r:id="rId22"/>
-    <sheet name="HyperlinkToUpdate" sheetId="17" r:id="rId23"/>
+    <sheet name="PivotChart" sheetId="27" r:id="rId17"/>
+    <sheet name="Sheet5" sheetId="30" r:id="rId18"/>
+    <sheet name="Sheet6" sheetId="31" r:id="rId19"/>
+    <sheet name="pivotTable" sheetId="28" r:id="rId20"/>
+    <sheet name="TableTotalRow" sheetId="21" r:id="rId21"/>
+    <sheet name="VlookupApproximatematch" sheetId="12" r:id="rId22"/>
+    <sheet name="LookupFullRecord" sheetId="13" r:id="rId23"/>
+    <sheet name="HyperlinkToWorksheet" sheetId="14" r:id="rId24"/>
+    <sheet name="HypelinkToFile" sheetId="15" r:id="rId25"/>
+    <sheet name="HyperlinkToWebpage" sheetId="16" r:id="rId26"/>
+    <sheet name="HyperlinkToUpdate" sheetId="17" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Filtering!$B$4:$E$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">VlookupApproximatematch!$A$3:$D$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">VlookupApproximatematch!$A$3:$D$8</definedName>
+    <definedName name="Slicer_Name">#N/A</definedName>
     <definedName name="vtable">VlookupDataValidationExact!$A$3:$D$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId28"/>
+    <pivotCache cacheId="10" r:id="rId29"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId30"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -80,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="211">
   <si>
     <t>Month</t>
   </si>
@@ -629,6 +646,90 @@
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Marker</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Projector</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>PenDrive</t>
+  </si>
+  <si>
+    <t>East</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>MidWest</t>
+  </si>
+  <si>
+    <t>Shahid</t>
+  </si>
+  <si>
+    <t>Tahia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazar </t>
+  </si>
+  <si>
+    <t>Kuddus</t>
+  </si>
+  <si>
+    <t>Sokina</t>
+  </si>
+  <si>
+    <t>Sobuj</t>
+  </si>
+  <si>
+    <t>Kusum</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Sum of Sales</t>
+  </si>
+  <si>
+    <t>(All)</t>
   </si>
 </sst>
 </file>
@@ -907,7 +1008,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1004,6 +1105,12 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1011,7 +1118,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4327,6 +4437,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1777619263"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4406,6 +4517,451 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[for job.xlsx]PivotChart!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$K$9:$K$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>East</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$J$11:$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Fazar </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feroza</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kuddus</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tahia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$K$11:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9778-4A3A-87E7-7A4C8DC0108A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PivotChart!$L$9:$L$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>West</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>PivotChart!$J$11:$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Fazar </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feroza</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kuddus</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Tahia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>PivotChart!$L$11:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-9778-4A3A-87E7-7A4C8DC0108A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="533730943"/>
+        <c:axId val="533732191"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="533730943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533732191"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533732191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533730943"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
 </c:chartSpace>
 </file>
 
@@ -4649,6 +5205,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
@@ -7248,6 +7844,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7960,6 +9059,118 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Name"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Name"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11153775" y="695325"/>
+              <a:ext cx="1828800" cy="2524125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -8017,14 +9228,683 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="44128.519555555555" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="13">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B4:G17" sheet="PivotChart"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-11-10T00:00:00" maxDate="2019-11-23T00:00:00" count="13">
+        <d v="2019-11-10T00:00:00"/>
+        <d v="2019-11-11T00:00:00"/>
+        <d v="2019-11-12T00:00:00"/>
+        <d v="2019-11-13T00:00:00"/>
+        <d v="2019-11-14T00:00:00"/>
+        <d v="2019-11-15T00:00:00"/>
+        <d v="2019-11-16T00:00:00"/>
+        <d v="2019-11-17T00:00:00"/>
+        <d v="2019-11-18T00:00:00"/>
+        <d v="2019-11-19T00:00:00"/>
+        <d v="2019-11-20T00:00:00"/>
+        <d v="2019-11-21T00:00:00"/>
+        <d v="2019-11-22T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Product" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Chair"/>
+        <s v="Table"/>
+        <s v="Board"/>
+        <s v="Marker"/>
+        <s v="laptop"/>
+        <s v="Projector"/>
+        <s v="Switch"/>
+        <s v="Lights"/>
+        <s v="Camera"/>
+        <s v="PenDrive"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="4">
+        <s v="East"/>
+        <s v="West"/>
+        <s v="south"/>
+        <s v="MidWest"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems count="13">
+        <s v="taj"/>
+        <s v="nazrul"/>
+        <s v="Shahid"/>
+        <s v="Kohinoor"/>
+        <s v="Tahia"/>
+        <s v="Fazar "/>
+        <s v="Rina"/>
+        <s v="Nurul"/>
+        <s v="Feroza"/>
+        <s v="Kuddus"/>
+        <s v="Sokina"/>
+        <s v="Sobuj"/>
+        <s v="Kusum"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Units" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15" maxValue="75"/>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="168">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="200" maxValue="800"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="44128.540571759258" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="13">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B4:G17" sheet="pivotTable"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-11-10T00:00:00" maxDate="2019-11-23T00:00:00"/>
+    </cacheField>
+    <cacheField name="Product" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Chair"/>
+        <s v="Table"/>
+        <s v="Board"/>
+        <s v="Marker"/>
+        <s v="laptop"/>
+        <s v="Projector"/>
+        <s v="Switch"/>
+        <s v="Lights"/>
+        <s v="Camera"/>
+        <s v="PenDrive"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="4">
+        <s v="East"/>
+        <s v="West"/>
+        <s v="south"/>
+        <s v="MidWest"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems count="13">
+        <s v="taj"/>
+        <s v="nazrul"/>
+        <s v="Shahid"/>
+        <s v="Kohinoor"/>
+        <s v="Tahia"/>
+        <s v="Fazar "/>
+        <s v="Rina"/>
+        <s v="Nurul"/>
+        <s v="Feroza"/>
+        <s v="Kuddus"/>
+        <s v="Sokina"/>
+        <s v="Sobuj"/>
+        <s v="Kusum"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Units" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="15" maxValue="75"/>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="168">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="200" maxValue="800"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="13">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="20"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="25"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="30"/>
+    <n v="350"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="35"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="40"/>
+    <n v="450"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="45"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="50"/>
+    <n v="550"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="55"/>
+    <n v="600"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="60"/>
+    <n v="650"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="10"/>
+    <n v="65"/>
+    <n v="700"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="11"/>
+    <n v="70"/>
+    <n v="750"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="12"/>
+    <n v="75"/>
+    <n v="800"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="13">
+  <r>
+    <d v="2019-11-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15"/>
+    <n v="200"/>
+  </r>
+  <r>
+    <d v="2019-11-11T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="20"/>
+    <n v="250"/>
+  </r>
+  <r>
+    <d v="2019-11-12T00:00:00"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="25"/>
+    <n v="300"/>
+  </r>
+  <r>
+    <d v="2019-11-13T00:00:00"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="30"/>
+    <n v="350"/>
+  </r>
+  <r>
+    <d v="2019-11-14T00:00:00"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="35"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <d v="2019-11-15T00:00:00"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="40"/>
+    <n v="450"/>
+  </r>
+  <r>
+    <d v="2019-11-16T00:00:00"/>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="45"/>
+    <n v="500"/>
+  </r>
+  <r>
+    <d v="2019-11-17T00:00:00"/>
+    <x v="7"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="50"/>
+    <n v="550"/>
+  </r>
+  <r>
+    <d v="2019-11-18T00:00:00"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="8"/>
+    <n v="55"/>
+    <n v="600"/>
+  </r>
+  <r>
+    <d v="2019-11-19T00:00:00"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="60"/>
+    <n v="650"/>
+  </r>
+  <r>
+    <d v="2019-11-20T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="10"/>
+    <n v="65"/>
+    <n v="700"/>
+  </r>
+  <r>
+    <d v="2019-11-21T00:00:00"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="11"/>
+    <n v="70"/>
+    <n v="750"/>
+  </r>
+  <r>
+    <d v="2019-11-22T00:00:00"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="12"/>
+    <n v="75"/>
+    <n v="800"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="J9:M15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisPage" numFmtId="14" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="11">
+        <item h="1" x="2"/>
+        <item x="8"/>
+        <item h="1" x="0"/>
+        <item x="4"/>
+        <item h="1" x="7"/>
+        <item h="1" x="3"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="14">
+        <item sd="0" x="5"/>
+        <item sd="0" x="8"/>
+        <item x="3"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="0"/>
+        <item t="default" sd="0"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="168" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K4:M7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="11">
+        <item x="2"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="14">
+        <item h="1" x="5"/>
+        <item h="1" x="8"/>
+        <item h="1" x="3"/>
+        <item h="1" x="9"/>
+        <item h="1" x="12"/>
+        <item x="1"/>
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="2"/>
+        <item h="1" x="11"/>
+        <item h="1" x="10"/>
+        <item h="1" x="4"/>
+        <item h="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="168" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="5" baseField="3" baseItem="0" numFmtId="168"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Name" sourceName="Name">
+  <pivotTables>
+    <pivotTable tabId="28" name="PivotTable2"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1">
+      <items count="13">
+        <i x="5"/>
+        <i x="8"/>
+        <i x="3"/>
+        <i x="9"/>
+        <i x="12"/>
+        <i x="1" s="1"/>
+        <i x="7"/>
+        <i x="6"/>
+        <i x="2"/>
+        <i x="11"/>
+        <i x="10"/>
+        <i x="4"/>
+        <i x="0"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Name" cache="Slicer_Name" caption="Name" startItem="5" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C4:F13" totalsRowCount="1" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Date" dataDxfId="0"/>
+    <tableColumn id="2" name="Product"/>
+    <tableColumn id="3" name="Region"/>
+    <tableColumn id="4" name="Name"/>
+    <tableColumn id="5" name="Units"/>
+    <tableColumn id="6" name="Sales"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Product"/>
+    <tableColumn id="3" name="Region"/>
+    <tableColumn id="4" name="Name"/>
+    <tableColumn id="5" name="Units"/>
+    <tableColumn id="6" name="Sales"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="C4:F13" totalsRowCount="1" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="C4:F12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Top Product" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="product code" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="Quantity" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="Price" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" name="Top Product" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="2" name="product code" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Quantity" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="Price" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9181,7 +11061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
@@ -9310,6 +11190,849 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="28"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>43779</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="10">
+        <v>15</v>
+      </c>
+      <c r="G5" s="63">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>43780</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="10">
+        <v>20</v>
+      </c>
+      <c r="G6" s="63">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>43781</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="10">
+        <v>25</v>
+      </c>
+      <c r="G7" s="63">
+        <v>300</v>
+      </c>
+      <c r="J7" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>43782</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="10">
+        <v>30</v>
+      </c>
+      <c r="G8" s="63">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>43783</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F9" s="10">
+        <v>35</v>
+      </c>
+      <c r="G9" s="63">
+        <v>400</v>
+      </c>
+      <c r="J9" s="73" t="s">
+        <v>209</v>
+      </c>
+      <c r="K9" s="73" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <v>43784</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="10">
+        <v>40</v>
+      </c>
+      <c r="G10" s="63">
+        <v>450</v>
+      </c>
+      <c r="J10" s="73" t="s">
+        <v>207</v>
+      </c>
+      <c r="K10" t="s">
+        <v>196</v>
+      </c>
+      <c r="L10" t="s">
+        <v>197</v>
+      </c>
+      <c r="M10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>43785</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="10">
+        <v>45</v>
+      </c>
+      <c r="G11" s="63">
+        <v>500</v>
+      </c>
+      <c r="J11" s="74" t="s">
+        <v>202</v>
+      </c>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75">
+        <v>450</v>
+      </c>
+      <c r="M11" s="75">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <v>43786</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="10">
+        <v>50</v>
+      </c>
+      <c r="G12" s="63">
+        <v>550</v>
+      </c>
+      <c r="J12" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="K12" s="75">
+        <v>600</v>
+      </c>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <v>43787</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="10">
+        <v>55</v>
+      </c>
+      <c r="G13" s="63">
+        <v>600</v>
+      </c>
+      <c r="J13" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75">
+        <v>650</v>
+      </c>
+      <c r="M13" s="75">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <v>43788</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="10">
+        <v>60</v>
+      </c>
+      <c r="G14" s="63">
+        <v>650</v>
+      </c>
+      <c r="J14" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="K14" s="75">
+        <v>400</v>
+      </c>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <v>43789</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="10">
+        <v>65</v>
+      </c>
+      <c r="G15" s="63">
+        <v>700</v>
+      </c>
+      <c r="J15" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="K15" s="75">
+        <v>1000</v>
+      </c>
+      <c r="L15" s="75">
+        <v>1100</v>
+      </c>
+      <c r="M15" s="75">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <v>43790</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="10">
+        <v>70</v>
+      </c>
+      <c r="G16" s="63">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <v>43791</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="10">
+        <v>75</v>
+      </c>
+      <c r="G17" s="63">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <v>43791</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="F2">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="6.85546875" customWidth="1"/>
+    <col min="27" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.85546875" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.7109375" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.5703125" customWidth="1"/>
+    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.5703125" customWidth="1"/>
+    <col min="37" max="37" width="8.140625" customWidth="1"/>
+    <col min="38" max="38" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="K4" s="73" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>43779</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="10">
+        <v>15</v>
+      </c>
+      <c r="G5" s="63">
+        <v>200</v>
+      </c>
+      <c r="L5" t="s">
+        <v>197</v>
+      </c>
+      <c r="M5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
+        <v>43780</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="10">
+        <v>20</v>
+      </c>
+      <c r="G6" s="63">
+        <v>250</v>
+      </c>
+      <c r="K6" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="28">
+        <v>250</v>
+      </c>
+      <c r="M6" s="28">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>43781</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="10">
+        <v>25</v>
+      </c>
+      <c r="G7" s="63">
+        <v>300</v>
+      </c>
+      <c r="K7" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="L7" s="28">
+        <v>250</v>
+      </c>
+      <c r="M7" s="28">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>43782</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="10">
+        <v>30</v>
+      </c>
+      <c r="G8" s="63">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>43783</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F9" s="10">
+        <v>35</v>
+      </c>
+      <c r="G9" s="63">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <v>43784</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="10">
+        <v>40</v>
+      </c>
+      <c r="G10" s="63">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>43785</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="10">
+        <v>45</v>
+      </c>
+      <c r="G11" s="63">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <v>43786</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="10">
+        <v>50</v>
+      </c>
+      <c r="G12" s="63">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <v>43787</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="10">
+        <v>55</v>
+      </c>
+      <c r="G13" s="63">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <v>43788</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="10">
+        <v>60</v>
+      </c>
+      <c r="G14" s="63">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <v>43789</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="10">
+        <v>65</v>
+      </c>
+      <c r="G15" s="63">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <v>43790</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="10">
+        <v>70</v>
+      </c>
+      <c r="G16" s="63">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <v>43791</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="10">
+        <v>75</v>
+      </c>
+      <c r="G17" s="63">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:F13"/>
   <sheetViews>
@@ -9471,435 +12194,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="29"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="10">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="10">
-        <v>2000</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="10">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="10">
-        <v>5000</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D7" s="10">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="10">
-        <v>10000</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="10">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
-        <v>4990</v>
-      </c>
-      <c r="B13">
-        <f>VLOOKUP(A13,B3:D8,3,1)</f>
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A3:D8"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" style="38" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="18" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="38"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>157</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="38" t="str">
-        <f>LOOKUP($A$17,$A$5:$A$13,B5:B13)</f>
-        <v xml:space="preserve">Rina </v>
-      </c>
-      <c r="C17" s="38" t="str">
-        <f t="shared" ref="C17:E17" si="0">LOOKUP($A$17,$A$5:$A$13,C5:C13)</f>
-        <v>Begum</v>
-      </c>
-      <c r="D17" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>taj@gmail.com</v>
-      </c>
-      <c r="E17" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>017-55459</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A17">
-      <formula1>$A$5:$A$13</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D6:D13" r:id="rId2" display="taj@gmail.com"/>
-    <hyperlink ref="D6" r:id="rId3"/>
-    <hyperlink ref="D7" r:id="rId4"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="34" t="s">
-        <v>167</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" location="LookupFullRecord!A4" display="Go to LookupFullRecord"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="34" t="s">
-        <v>168</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10059,6 +12353,435 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="29"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="10">
+        <v>10000</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="28">
+        <v>4990</v>
+      </c>
+      <c r="B13">
+        <f>VLOOKUP(A13,B3:D8,3,1)</f>
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:D8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" style="38" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="18" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="38" t="str">
+        <f>LOOKUP($A$17,$A$5:$A$13,B5:B13)</f>
+        <v xml:space="preserve">Rina </v>
+      </c>
+      <c r="C17" s="38" t="str">
+        <f t="shared" ref="C17:E17" si="0">LOOKUP($A$17,$A$5:$A$13,C5:C13)</f>
+        <v>Begum</v>
+      </c>
+      <c r="D17" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>taj@gmail.com</v>
+      </c>
+      <c r="E17" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>017-55459</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A17">
+      <formula1>$A$5:$A$13</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D6:D13" r:id="rId2" display="taj@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D7" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" location="LookupFullRecord!A4" display="Go to LookupFullRecord"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10103,7 +12826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3"/>
   <sheetViews>
@@ -10437,7 +13160,7 @@
       </c>
       <c r="F14" s="11">
         <f ca="1">IF(E4&lt;F4,TODAY(),TODAY()+10)</f>
-        <v>44137</v>
+        <v>44138</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>